<commit_message>
New figures new data
</commit_message>
<xml_diff>
--- a/data/fem/modelinput-f28.xlsx
+++ b/data/fem/modelinput-f28.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:M70"/>
+  <dimension ref="A1:M62"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2303,7 +2303,7 @@
     </row>
     <row r="44">
       <c r="A44" s="1" t="n">
-        <v>460</v>
+        <v>468</v>
       </c>
       <c r="B44" t="inlineStr">
         <is>
@@ -2314,39 +2314,39 @@
         <v>1</v>
       </c>
       <c r="D44" t="n">
-        <v>0.7226272727272728</v>
+        <v>2.116846666666667</v>
       </c>
       <c r="E44" t="n">
-        <v>0.02294485607831405</v>
+        <v>0.02487560407630172</v>
       </c>
       <c r="F44" t="n">
         <v>1200</v>
       </c>
       <c r="G44" t="n">
-        <v>0.8346618181818183</v>
+        <v>2.507571384615385</v>
       </c>
       <c r="H44" t="n">
-        <v>0.02672938719614563</v>
+        <v>0.03126460830298725</v>
       </c>
       <c r="I44" t="n">
-        <v>21.21386763088215</v>
+        <v>23.80128702367193</v>
       </c>
       <c r="J44" t="n">
-        <v>20.09805</v>
+        <v>20.20757</v>
       </c>
       <c r="K44" t="n">
-        <v>20.03732</v>
+        <v>20.03889999999999</v>
       </c>
       <c r="L44" t="n">
-        <v>19.67285</v>
+        <v>19.73873</v>
       </c>
       <c r="M44" t="n">
-        <v>19.67998</v>
+        <v>19.73965</v>
       </c>
     </row>
     <row r="45">
       <c r="A45" s="1" t="n">
-        <v>461</v>
+        <v>469</v>
       </c>
       <c r="B45" t="inlineStr">
         <is>
@@ -2357,39 +2357,39 @@
         <v>1</v>
       </c>
       <c r="D45" t="n">
-        <v>0.5348611111111111</v>
+        <v>2.102648275862069</v>
       </c>
       <c r="E45" t="n">
-        <v>0.01291279050903245</v>
+        <v>0.02521989889933365</v>
       </c>
       <c r="F45" t="n">
         <v>1200</v>
       </c>
       <c r="G45" t="n">
-        <v>0.6113024242424242</v>
+        <v>2.49070078817734</v>
       </c>
       <c r="H45" t="n">
-        <v>0.01497644708708993</v>
+        <v>0.03162557828544835</v>
       </c>
       <c r="I45" t="n">
-        <v>21.07872252645977</v>
+        <v>23.76461996489986</v>
       </c>
       <c r="J45" t="n">
-        <v>20.08738</v>
+        <v>20.22325</v>
       </c>
       <c r="K45" t="n">
-        <v>20.04362</v>
+        <v>20.03421</v>
       </c>
       <c r="L45" t="n">
-        <v>19.74565</v>
+        <v>19.72448</v>
       </c>
       <c r="M45" t="n">
-        <v>19.71476</v>
+        <v>19.74222</v>
       </c>
     </row>
     <row r="46">
       <c r="A46" s="1" t="n">
-        <v>462</v>
+        <v>470</v>
       </c>
       <c r="B46" t="inlineStr">
         <is>
@@ -2400,39 +2400,39 @@
         <v>1</v>
       </c>
       <c r="D46" t="n">
-        <v>0.5242545454545454</v>
+        <v>2.071419230769231</v>
       </c>
       <c r="E46" t="n">
-        <v>0.01008318807809227</v>
+        <v>0.02021300609470584</v>
       </c>
       <c r="F46" t="n">
         <v>1200</v>
       </c>
       <c r="G46" t="n">
-        <v>0.5965399373040753</v>
+        <v>2.444824816053512</v>
       </c>
       <c r="H46" t="n">
-        <v>0.01173962867714591</v>
+        <v>0.02594056958700109</v>
       </c>
       <c r="I46" t="n">
-        <v>21.06999718832315</v>
+        <v>23.77079895683795</v>
       </c>
       <c r="J46" t="n">
-        <v>20.06988</v>
+        <v>20.2234</v>
       </c>
       <c r="K46" t="n">
-        <v>20.05483</v>
+        <v>20.03177</v>
       </c>
       <c r="L46" t="n">
-        <v>19.65171</v>
+        <v>19.67224</v>
       </c>
       <c r="M46" t="n">
-        <v>19.75817</v>
+        <v>19.68673</v>
       </c>
     </row>
     <row r="47">
       <c r="A47" s="1" t="n">
-        <v>463</v>
+        <v>471</v>
       </c>
       <c r="B47" t="inlineStr">
         <is>
@@ -2443,39 +2443,39 @@
         <v>1</v>
       </c>
       <c r="D47" t="n">
-        <v>0.4993939393939394</v>
+        <v>29.76260370370371</v>
       </c>
       <c r="E47" t="n">
-        <v>0.01406240420842796</v>
+        <v>0.1799391253505171</v>
       </c>
       <c r="F47" t="n">
         <v>1200</v>
       </c>
       <c r="G47" t="n">
-        <v>0.5629927272727273</v>
+        <v>35.61187194444445</v>
       </c>
       <c r="H47" t="n">
-        <v>0.01602589270774393</v>
+        <v>0.2614817586619869</v>
       </c>
       <c r="I47" t="n">
-        <v>20.97424421495006</v>
+        <v>27.76417257216145</v>
       </c>
       <c r="J47" t="n">
-        <v>20.07217</v>
+        <v>20.42233</v>
       </c>
       <c r="K47" t="n">
-        <v>20.03788</v>
+        <v>20.03725</v>
       </c>
       <c r="L47" t="n">
-        <v>19.73618</v>
+        <v>19.73922</v>
       </c>
       <c r="M47" t="n">
-        <v>19.74196</v>
+        <v>19.7161</v>
       </c>
     </row>
     <row r="48">
       <c r="A48" s="1" t="n">
-        <v>464</v>
+        <v>472</v>
       </c>
       <c r="B48" t="inlineStr">
         <is>
@@ -2486,39 +2486,39 @@
         <v>1</v>
       </c>
       <c r="D48" t="n">
-        <v>0.4845787878787878</v>
+        <v>30.26423636363636</v>
       </c>
       <c r="E48" t="n">
-        <v>0.01266670728661748</v>
+        <v>0.1128262848163245</v>
       </c>
       <c r="F48" t="n">
         <v>1200</v>
       </c>
       <c r="G48" t="n">
-        <v>0.5485527272727271</v>
+        <v>36.17695999999999</v>
       </c>
       <c r="H48" t="n">
-        <v>0.01451998501916403</v>
+        <v>0.2022657477161512</v>
       </c>
       <c r="I48" t="n">
-        <v>20.99566124135685</v>
+        <v>27.95957988159558</v>
       </c>
       <c r="J48" t="n">
-        <v>20.06767</v>
+        <v>20.42206</v>
       </c>
       <c r="K48" t="n">
-        <v>20.03789</v>
+        <v>20.0415</v>
       </c>
       <c r="L48" t="n">
-        <v>19.69799</v>
+        <v>19.73344</v>
       </c>
       <c r="M48" t="n">
-        <v>19.73221</v>
+        <v>19.7478</v>
       </c>
     </row>
     <row r="49">
       <c r="A49" s="1" t="n">
-        <v>465</v>
+        <v>473</v>
       </c>
       <c r="B49" t="inlineStr">
         <is>
@@ -2529,39 +2529,39 @@
         <v>1</v>
       </c>
       <c r="D49" t="n">
-        <v>1.005315151515151</v>
+        <v>41.35133</v>
       </c>
       <c r="E49" t="n">
-        <v>0.0153122524717161</v>
+        <v>0.3535965279178451</v>
       </c>
       <c r="F49" t="n">
         <v>1200</v>
       </c>
       <c r="G49" t="n">
-        <v>1.170283636363636</v>
+        <v>49.498556</v>
       </c>
       <c r="H49" t="n">
-        <v>0.01847986747867087</v>
+        <v>0.4708383509652719</v>
       </c>
       <c r="I49" t="n">
-        <v>21.94716764104016</v>
+        <v>30.38313213379842</v>
       </c>
       <c r="J49" t="n">
-        <v>20.12795999999999</v>
+        <v>20.53963</v>
       </c>
       <c r="K49" t="n">
-        <v>20.04119</v>
+        <v>20.04528</v>
       </c>
       <c r="L49" t="n">
-        <v>19.72443</v>
+        <v>19.71651</v>
       </c>
       <c r="M49" t="n">
-        <v>19.72606</v>
+        <v>19.73258</v>
       </c>
     </row>
     <row r="50">
       <c r="A50" s="1" t="n">
-        <v>466</v>
+        <v>474</v>
       </c>
       <c r="B50" t="inlineStr">
         <is>
@@ -2572,39 +2572,39 @@
         <v>1</v>
       </c>
       <c r="D50" t="n">
-        <v>1.010818181818182</v>
+        <v>47.15725882352942</v>
       </c>
       <c r="E50" t="n">
-        <v>0.01316326456814225</v>
+        <v>0.33274548655621</v>
       </c>
       <c r="F50" t="n">
         <v>1200</v>
       </c>
       <c r="G50" t="n">
-        <v>1.161741818181818</v>
+        <v>56.4736196791444</v>
       </c>
       <c r="H50" t="n">
-        <v>0.01588418659958593</v>
+        <v>0.4627716101616476</v>
       </c>
       <c r="I50" t="n">
-        <v>21.85090020455242</v>
+        <v>31.81152450793848</v>
       </c>
       <c r="J50" t="n">
-        <v>20.12883</v>
+        <v>20.60683</v>
       </c>
       <c r="K50" t="n">
-        <v>20.04297</v>
+        <v>20.03405</v>
       </c>
       <c r="L50" t="n">
-        <v>19.74553</v>
+        <v>19.73644</v>
       </c>
       <c r="M50" t="n">
-        <v>19.72435</v>
+        <v>19.74915</v>
       </c>
     </row>
     <row r="51">
       <c r="A51" s="1" t="n">
-        <v>467</v>
+        <v>475</v>
       </c>
       <c r="B51" t="inlineStr">
         <is>
@@ -2615,39 +2615,39 @@
         <v>1</v>
       </c>
       <c r="D51" t="n">
-        <v>1.010854545454545</v>
+        <v>59.215</v>
       </c>
       <c r="E51" t="n">
-        <v>0.01162255595031408</v>
+        <v>0.4292151907842963</v>
       </c>
       <c r="F51" t="n">
         <v>1200</v>
       </c>
       <c r="G51" t="n">
-        <v>1.175866993006992</v>
+        <v>71.07653454545455</v>
       </c>
       <c r="H51" t="n">
-        <v>0.01438020608797658</v>
+        <v>0.5942470287417343</v>
       </c>
       <c r="I51" t="n">
-        <v>22.01222794042024</v>
+        <v>35.03853174687898</v>
       </c>
       <c r="J51" t="n">
-        <v>20.12776</v>
+        <v>20.75381</v>
       </c>
       <c r="K51" t="n">
-        <v>20.04385</v>
+        <v>20.03718</v>
       </c>
       <c r="L51" t="n">
-        <v>19.73305</v>
+        <v>19.73597</v>
       </c>
       <c r="M51" t="n">
-        <v>19.69665</v>
+        <v>19.72144</v>
       </c>
     </row>
     <row r="52">
       <c r="A52" s="1" t="n">
-        <v>468</v>
+        <v>476</v>
       </c>
       <c r="B52" t="inlineStr">
         <is>
@@ -2658,39 +2658,39 @@
         <v>1</v>
       </c>
       <c r="D52" t="n">
-        <v>2.116846666666667</v>
+        <v>102.13665</v>
       </c>
       <c r="E52" t="n">
-        <v>0.02487560407630172</v>
+        <v>1.093682058461236</v>
       </c>
       <c r="F52" t="n">
         <v>1200</v>
       </c>
       <c r="G52" t="n">
-        <v>2.507571384615385</v>
+        <v>122.43535125</v>
       </c>
       <c r="H52" t="n">
-        <v>0.03126460830298725</v>
+        <v>1.406797446867239</v>
       </c>
       <c r="I52" t="n">
-        <v>23.80128702367193</v>
+        <v>54.14499303081595</v>
       </c>
       <c r="J52" t="n">
-        <v>20.20757</v>
+        <v>21.34346</v>
       </c>
       <c r="K52" t="n">
-        <v>20.03889999999999</v>
+        <v>20.03454</v>
       </c>
       <c r="L52" t="n">
-        <v>19.73873</v>
+        <v>19.76377</v>
       </c>
       <c r="M52" t="n">
-        <v>19.73965</v>
+        <v>19.65336</v>
       </c>
     </row>
     <row r="53">
       <c r="A53" s="1" t="n">
-        <v>469</v>
+        <v>477</v>
       </c>
       <c r="B53" t="inlineStr">
         <is>
@@ -2701,39 +2701,39 @@
         <v>1</v>
       </c>
       <c r="D53" t="n">
-        <v>2.102648275862069</v>
+        <v>108.9872333333333</v>
       </c>
       <c r="E53" t="n">
-        <v>0.02521989889933365</v>
+        <v>0.2327150245829983</v>
       </c>
       <c r="F53" t="n">
         <v>1200</v>
       </c>
       <c r="G53" t="n">
-        <v>2.49070078817734</v>
+        <v>130.6417286956521</v>
       </c>
       <c r="H53" t="n">
-        <v>0.03162557828544835</v>
+        <v>0.6116545429652889</v>
       </c>
       <c r="I53" t="n">
-        <v>23.76461996489986</v>
+        <v>55.53830622830953</v>
       </c>
       <c r="J53" t="n">
-        <v>20.22325</v>
+        <v>21.38578</v>
       </c>
       <c r="K53" t="n">
-        <v>20.03421</v>
+        <v>20.03494</v>
       </c>
       <c r="L53" t="n">
-        <v>19.72448</v>
+        <v>19.75404</v>
       </c>
       <c r="M53" t="n">
-        <v>19.74222</v>
+        <v>19.73946</v>
       </c>
     </row>
     <row r="54">
       <c r="A54" s="1" t="n">
-        <v>470</v>
+        <v>478</v>
       </c>
       <c r="B54" t="inlineStr">
         <is>
@@ -2744,39 +2744,39 @@
         <v>1</v>
       </c>
       <c r="D54" t="n">
-        <v>2.071419230769231</v>
+        <v>112.97665</v>
       </c>
       <c r="E54" t="n">
-        <v>0.02021300609470584</v>
+        <v>0.7234093357152652</v>
       </c>
       <c r="F54" t="n">
         <v>1200</v>
       </c>
       <c r="G54" t="n">
-        <v>2.444824816053512</v>
+        <v>135.41718</v>
       </c>
       <c r="H54" t="n">
-        <v>0.02594056958700109</v>
+        <v>1.03451785756271</v>
       </c>
       <c r="I54" t="n">
-        <v>23.77079895683795</v>
+        <v>57.04827480188973</v>
       </c>
       <c r="J54" t="n">
-        <v>20.2234</v>
+        <v>21.4083</v>
       </c>
       <c r="K54" t="n">
-        <v>20.03177</v>
+        <v>20.03928</v>
       </c>
       <c r="L54" t="n">
-        <v>19.67224</v>
+        <v>19.73125</v>
       </c>
       <c r="M54" t="n">
-        <v>19.68673</v>
+        <v>19.68085</v>
       </c>
     </row>
     <row r="55">
       <c r="A55" s="1" t="n">
-        <v>471</v>
+        <v>480</v>
       </c>
       <c r="B55" t="inlineStr">
         <is>
@@ -2787,39 +2787,39 @@
         <v>1</v>
       </c>
       <c r="D55" t="n">
-        <v>29.76260370370371</v>
+        <v>88.27258888888886</v>
       </c>
       <c r="E55" t="n">
-        <v>0.1799391253505171</v>
+        <v>0.2792710038853143</v>
       </c>
       <c r="F55" t="n">
         <v>1200</v>
       </c>
       <c r="G55" t="n">
-        <v>35.61187194444445</v>
+        <v>105.7975212121212</v>
       </c>
       <c r="H55" t="n">
-        <v>0.2614817586619869</v>
+        <v>0.5534972515446569</v>
       </c>
       <c r="I55" t="n">
-        <v>27.76417257216145</v>
+        <v>45.12128775795832</v>
       </c>
       <c r="J55" t="n">
-        <v>20.42233</v>
+        <v>21.08996</v>
       </c>
       <c r="K55" t="n">
-        <v>20.03725</v>
+        <v>20.04585</v>
       </c>
       <c r="L55" t="n">
-        <v>19.73922</v>
+        <v>19.7502</v>
       </c>
       <c r="M55" t="n">
-        <v>19.7161</v>
+        <v>19.75275</v>
       </c>
     </row>
     <row r="56">
       <c r="A56" s="1" t="n">
-        <v>472</v>
+        <v>481</v>
       </c>
       <c r="B56" t="inlineStr">
         <is>
@@ -2830,39 +2830,39 @@
         <v>1</v>
       </c>
       <c r="D56" t="n">
-        <v>30.26423636363636</v>
+        <v>75.07555333333333</v>
       </c>
       <c r="E56" t="n">
-        <v>0.1128262848163245</v>
+        <v>0.2830642528439352</v>
       </c>
       <c r="F56" t="n">
         <v>1200</v>
       </c>
       <c r="G56" t="n">
-        <v>36.17695999999999</v>
+        <v>90.030928</v>
       </c>
       <c r="H56" t="n">
-        <v>0.2022657477161512</v>
+        <v>0.5059142637266609</v>
       </c>
       <c r="I56" t="n">
-        <v>27.95957988159558</v>
+        <v>40.31496211839858</v>
       </c>
       <c r="J56" t="n">
-        <v>20.42206</v>
+        <v>20.93419</v>
       </c>
       <c r="K56" t="n">
-        <v>20.0415</v>
+        <v>20.03498</v>
       </c>
       <c r="L56" t="n">
-        <v>19.73344</v>
+        <v>19.73728</v>
       </c>
       <c r="M56" t="n">
-        <v>19.7478</v>
+        <v>19.70217</v>
       </c>
     </row>
     <row r="57">
       <c r="A57" s="1" t="n">
-        <v>473</v>
+        <v>482</v>
       </c>
       <c r="B57" t="inlineStr">
         <is>
@@ -2873,39 +2873,39 @@
         <v>1</v>
       </c>
       <c r="D57" t="n">
-        <v>41.35133</v>
+        <v>76.63134000000001</v>
       </c>
       <c r="E57" t="n">
-        <v>0.3535965279178451</v>
+        <v>0.3919840393576105</v>
       </c>
       <c r="F57" t="n">
         <v>1200</v>
       </c>
       <c r="G57" t="n">
-        <v>49.498556</v>
+        <v>91.81433163636366</v>
       </c>
       <c r="H57" t="n">
-        <v>0.4708383509652719</v>
+        <v>0.6057401612922336</v>
       </c>
       <c r="I57" t="n">
-        <v>30.38313213379842</v>
+        <v>40.26403604613978</v>
       </c>
       <c r="J57" t="n">
-        <v>20.53963</v>
+        <v>20.94483</v>
       </c>
       <c r="K57" t="n">
-        <v>20.04528</v>
+        <v>20.03796</v>
       </c>
       <c r="L57" t="n">
-        <v>19.71651</v>
+        <v>19.72206</v>
       </c>
       <c r="M57" t="n">
-        <v>19.73258</v>
+        <v>19.72744</v>
       </c>
     </row>
     <row r="58">
       <c r="A58" s="1" t="n">
-        <v>474</v>
+        <v>483</v>
       </c>
       <c r="B58" t="inlineStr">
         <is>
@@ -2916,39 +2916,39 @@
         <v>1</v>
       </c>
       <c r="D58" t="n">
-        <v>47.15725882352942</v>
+        <v>78.38743846153847</v>
       </c>
       <c r="E58" t="n">
-        <v>0.33274548655621</v>
+        <v>0.438835499814493</v>
       </c>
       <c r="F58" t="n">
         <v>1200</v>
       </c>
       <c r="G58" t="n">
-        <v>56.4736196791444</v>
+        <v>93.92456251748253</v>
       </c>
       <c r="H58" t="n">
-        <v>0.4627716101616476</v>
+        <v>0.6554692731194366</v>
       </c>
       <c r="I58" t="n">
-        <v>31.81152450793848</v>
+        <v>40.86333081895141</v>
       </c>
       <c r="J58" t="n">
-        <v>20.60683</v>
+        <v>20.97386</v>
       </c>
       <c r="K58" t="n">
-        <v>20.03405</v>
+        <v>20.03447</v>
       </c>
       <c r="L58" t="n">
-        <v>19.73644</v>
+        <v>19.75148</v>
       </c>
       <c r="M58" t="n">
-        <v>19.74915</v>
+        <v>19.72307</v>
       </c>
     </row>
     <row r="59">
       <c r="A59" s="1" t="n">
-        <v>475</v>
+        <v>484</v>
       </c>
       <c r="B59" t="inlineStr">
         <is>
@@ -2959,39 +2959,39 @@
         <v>1</v>
       </c>
       <c r="D59" t="n">
-        <v>59.215</v>
+        <v>79.59875000000001</v>
       </c>
       <c r="E59" t="n">
-        <v>0.4292151907842963</v>
+        <v>0.1769806526956285</v>
       </c>
       <c r="F59" t="n">
         <v>1200</v>
       </c>
       <c r="G59" t="n">
-        <v>71.07653454545455</v>
+        <v>95.18118000000003</v>
       </c>
       <c r="H59" t="n">
-        <v>0.5942470287417343</v>
+        <v>0.4495198940511383</v>
       </c>
       <c r="I59" t="n">
-        <v>35.03853174687898</v>
+        <v>41.27421264811215</v>
       </c>
       <c r="J59" t="n">
-        <v>20.75381</v>
+        <v>20.9871</v>
       </c>
       <c r="K59" t="n">
-        <v>20.03718</v>
+        <v>20.04344</v>
       </c>
       <c r="L59" t="n">
-        <v>19.73597</v>
+        <v>19.73285</v>
       </c>
       <c r="M59" t="n">
-        <v>19.72144</v>
+        <v>19.7015</v>
       </c>
     </row>
     <row r="60">
       <c r="A60" s="1" t="n">
-        <v>476</v>
+        <v>485</v>
       </c>
       <c r="B60" t="inlineStr">
         <is>
@@ -3002,39 +3002,39 @@
         <v>1</v>
       </c>
       <c r="D60" t="n">
-        <v>102.13665</v>
+        <v>80.11731999999999</v>
       </c>
       <c r="E60" t="n">
-        <v>1.093682058461236</v>
+        <v>0.09281924369439799</v>
       </c>
       <c r="F60" t="n">
         <v>1200</v>
       </c>
       <c r="G60" t="n">
-        <v>122.43535125</v>
+        <v>96.243279</v>
       </c>
       <c r="H60" t="n">
-        <v>1.406797446867239</v>
+        <v>0.4162266416259908</v>
       </c>
       <c r="I60" t="n">
-        <v>54.14499303081595</v>
+        <v>41.34926437064848</v>
       </c>
       <c r="J60" t="n">
-        <v>21.34346</v>
+        <v>20.98686</v>
       </c>
       <c r="K60" t="n">
-        <v>20.03454</v>
+        <v>20.03783</v>
       </c>
       <c r="L60" t="n">
-        <v>19.76377</v>
+        <v>19.74506</v>
       </c>
       <c r="M60" t="n">
-        <v>19.65336</v>
+        <v>19.71404</v>
       </c>
     </row>
     <row r="61">
       <c r="A61" s="1" t="n">
-        <v>477</v>
+        <v>486</v>
       </c>
       <c r="B61" t="inlineStr">
         <is>
@@ -3045,39 +3045,39 @@
         <v>1</v>
       </c>
       <c r="D61" t="n">
-        <v>108.9872333333333</v>
+        <v>122.4533285714286</v>
       </c>
       <c r="E61" t="n">
-        <v>0.2327150245829983</v>
+        <v>0.05003850898010705</v>
       </c>
       <c r="F61" t="n">
         <v>1200</v>
       </c>
       <c r="G61" t="n">
-        <v>130.6417286956521</v>
+        <v>146.813197922078</v>
       </c>
       <c r="H61" t="n">
-        <v>0.6116545429652889</v>
+        <v>0.6146564231277903</v>
       </c>
       <c r="I61" t="n">
-        <v>55.53830622830953</v>
+        <v>59.80396282066845</v>
       </c>
       <c r="J61" t="n">
-        <v>21.38578</v>
+        <v>21.47603</v>
       </c>
       <c r="K61" t="n">
-        <v>20.03494</v>
+        <v>20.04177</v>
       </c>
       <c r="L61" t="n">
-        <v>19.75404</v>
+        <v>19.75535</v>
       </c>
       <c r="M61" t="n">
-        <v>19.73946</v>
+        <v>19.7496</v>
       </c>
     </row>
     <row r="62">
       <c r="A62" s="1" t="n">
-        <v>478</v>
+        <v>487</v>
       </c>
       <c r="B62" t="inlineStr">
         <is>
@@ -3088,377 +3088,33 @@
         <v>1</v>
       </c>
       <c r="D62" t="n">
-        <v>112.97665</v>
+        <v>126.1377666666667</v>
       </c>
       <c r="E62" t="n">
-        <v>0.7234093357152652</v>
+        <v>0.2602581077827704</v>
       </c>
       <c r="F62" t="n">
         <v>1200</v>
       </c>
       <c r="G62" t="n">
-        <v>135.41718</v>
+        <v>151.2493100000001</v>
       </c>
       <c r="H62" t="n">
-        <v>1.03451785756271</v>
+        <v>0.7032402392548338</v>
       </c>
       <c r="I62" t="n">
-        <v>57.04827480188973</v>
+        <v>60.54266808444977</v>
       </c>
       <c r="J62" t="n">
-        <v>21.4083</v>
+        <v>21.52416</v>
       </c>
       <c r="K62" t="n">
-        <v>20.03928</v>
+        <v>20.03652</v>
       </c>
       <c r="L62" t="n">
-        <v>19.73125</v>
+        <v>19.73887</v>
       </c>
       <c r="M62" t="n">
-        <v>19.68085</v>
-      </c>
-    </row>
-    <row r="63">
-      <c r="A63" s="1" t="n">
-        <v>480</v>
-      </c>
-      <c r="B63" t="inlineStr">
-        <is>
-          <t>f28</t>
-        </is>
-      </c>
-      <c r="C63" t="n">
-        <v>1</v>
-      </c>
-      <c r="D63" t="n">
-        <v>88.27258888888886</v>
-      </c>
-      <c r="E63" t="n">
-        <v>0.2792710038853143</v>
-      </c>
-      <c r="F63" t="n">
-        <v>1200</v>
-      </c>
-      <c r="G63" t="n">
-        <v>105.7975212121212</v>
-      </c>
-      <c r="H63" t="n">
-        <v>0.5534972515446569</v>
-      </c>
-      <c r="I63" t="n">
-        <v>45.12128775795832</v>
-      </c>
-      <c r="J63" t="n">
-        <v>21.08996</v>
-      </c>
-      <c r="K63" t="n">
-        <v>20.04585</v>
-      </c>
-      <c r="L63" t="n">
-        <v>19.7502</v>
-      </c>
-      <c r="M63" t="n">
-        <v>19.75275</v>
-      </c>
-    </row>
-    <row r="64">
-      <c r="A64" s="1" t="n">
-        <v>481</v>
-      </c>
-      <c r="B64" t="inlineStr">
-        <is>
-          <t>f28</t>
-        </is>
-      </c>
-      <c r="C64" t="n">
-        <v>1</v>
-      </c>
-      <c r="D64" t="n">
-        <v>75.07555333333333</v>
-      </c>
-      <c r="E64" t="n">
-        <v>0.2830642528439352</v>
-      </c>
-      <c r="F64" t="n">
-        <v>1200</v>
-      </c>
-      <c r="G64" t="n">
-        <v>90.030928</v>
-      </c>
-      <c r="H64" t="n">
-        <v>0.5059142637266609</v>
-      </c>
-      <c r="I64" t="n">
-        <v>40.31496211839858</v>
-      </c>
-      <c r="J64" t="n">
-        <v>20.93419</v>
-      </c>
-      <c r="K64" t="n">
-        <v>20.03498</v>
-      </c>
-      <c r="L64" t="n">
-        <v>19.73728</v>
-      </c>
-      <c r="M64" t="n">
-        <v>19.70217</v>
-      </c>
-    </row>
-    <row r="65">
-      <c r="A65" s="1" t="n">
-        <v>482</v>
-      </c>
-      <c r="B65" t="inlineStr">
-        <is>
-          <t>f28</t>
-        </is>
-      </c>
-      <c r="C65" t="n">
-        <v>1</v>
-      </c>
-      <c r="D65" t="n">
-        <v>76.63134000000001</v>
-      </c>
-      <c r="E65" t="n">
-        <v>0.3919840393576105</v>
-      </c>
-      <c r="F65" t="n">
-        <v>1200</v>
-      </c>
-      <c r="G65" t="n">
-        <v>91.81433163636366</v>
-      </c>
-      <c r="H65" t="n">
-        <v>0.6057401612922336</v>
-      </c>
-      <c r="I65" t="n">
-        <v>40.26403604613978</v>
-      </c>
-      <c r="J65" t="n">
-        <v>20.94483</v>
-      </c>
-      <c r="K65" t="n">
-        <v>20.03796</v>
-      </c>
-      <c r="L65" t="n">
-        <v>19.72206</v>
-      </c>
-      <c r="M65" t="n">
-        <v>19.72744</v>
-      </c>
-    </row>
-    <row r="66">
-      <c r="A66" s="1" t="n">
-        <v>483</v>
-      </c>
-      <c r="B66" t="inlineStr">
-        <is>
-          <t>f28</t>
-        </is>
-      </c>
-      <c r="C66" t="n">
-        <v>1</v>
-      </c>
-      <c r="D66" t="n">
-        <v>78.38743846153847</v>
-      </c>
-      <c r="E66" t="n">
-        <v>0.438835499814493</v>
-      </c>
-      <c r="F66" t="n">
-        <v>1200</v>
-      </c>
-      <c r="G66" t="n">
-        <v>93.92456251748253</v>
-      </c>
-      <c r="H66" t="n">
-        <v>0.6554692731194366</v>
-      </c>
-      <c r="I66" t="n">
-        <v>40.86333081895141</v>
-      </c>
-      <c r="J66" t="n">
-        <v>20.97386</v>
-      </c>
-      <c r="K66" t="n">
-        <v>20.03447</v>
-      </c>
-      <c r="L66" t="n">
-        <v>19.75148</v>
-      </c>
-      <c r="M66" t="n">
-        <v>19.72307</v>
-      </c>
-    </row>
-    <row r="67">
-      <c r="A67" s="1" t="n">
-        <v>484</v>
-      </c>
-      <c r="B67" t="inlineStr">
-        <is>
-          <t>f28</t>
-        </is>
-      </c>
-      <c r="C67" t="n">
-        <v>1</v>
-      </c>
-      <c r="D67" t="n">
-        <v>79.59875000000001</v>
-      </c>
-      <c r="E67" t="n">
-        <v>0.1769806526956285</v>
-      </c>
-      <c r="F67" t="n">
-        <v>1200</v>
-      </c>
-      <c r="G67" t="n">
-        <v>95.18118000000003</v>
-      </c>
-      <c r="H67" t="n">
-        <v>0.4495198940511383</v>
-      </c>
-      <c r="I67" t="n">
-        <v>41.27421264811215</v>
-      </c>
-      <c r="J67" t="n">
-        <v>20.9871</v>
-      </c>
-      <c r="K67" t="n">
-        <v>20.04344</v>
-      </c>
-      <c r="L67" t="n">
-        <v>19.73285</v>
-      </c>
-      <c r="M67" t="n">
-        <v>19.7015</v>
-      </c>
-    </row>
-    <row r="68">
-      <c r="A68" s="1" t="n">
-        <v>485</v>
-      </c>
-      <c r="B68" t="inlineStr">
-        <is>
-          <t>f28</t>
-        </is>
-      </c>
-      <c r="C68" t="n">
-        <v>1</v>
-      </c>
-      <c r="D68" t="n">
-        <v>80.11731999999999</v>
-      </c>
-      <c r="E68" t="n">
-        <v>0.09281924369439799</v>
-      </c>
-      <c r="F68" t="n">
-        <v>1200</v>
-      </c>
-      <c r="G68" t="n">
-        <v>96.243279</v>
-      </c>
-      <c r="H68" t="n">
-        <v>0.4162266416259908</v>
-      </c>
-      <c r="I68" t="n">
-        <v>41.34926437064848</v>
-      </c>
-      <c r="J68" t="n">
-        <v>20.98686</v>
-      </c>
-      <c r="K68" t="n">
-        <v>20.03783</v>
-      </c>
-      <c r="L68" t="n">
-        <v>19.74506</v>
-      </c>
-      <c r="M68" t="n">
-        <v>19.71404</v>
-      </c>
-    </row>
-    <row r="69">
-      <c r="A69" s="1" t="n">
-        <v>486</v>
-      </c>
-      <c r="B69" t="inlineStr">
-        <is>
-          <t>f28</t>
-        </is>
-      </c>
-      <c r="C69" t="n">
-        <v>1</v>
-      </c>
-      <c r="D69" t="n">
-        <v>122.4533285714286</v>
-      </c>
-      <c r="E69" t="n">
-        <v>0.05003850898010705</v>
-      </c>
-      <c r="F69" t="n">
-        <v>1200</v>
-      </c>
-      <c r="G69" t="n">
-        <v>146.813197922078</v>
-      </c>
-      <c r="H69" t="n">
-        <v>0.6146564231277903</v>
-      </c>
-      <c r="I69" t="n">
-        <v>59.80396282066845</v>
-      </c>
-      <c r="J69" t="n">
-        <v>21.47603</v>
-      </c>
-      <c r="K69" t="n">
-        <v>20.04177</v>
-      </c>
-      <c r="L69" t="n">
-        <v>19.75535</v>
-      </c>
-      <c r="M69" t="n">
-        <v>19.7496</v>
-      </c>
-    </row>
-    <row r="70">
-      <c r="A70" s="1" t="n">
-        <v>487</v>
-      </c>
-      <c r="B70" t="inlineStr">
-        <is>
-          <t>f28</t>
-        </is>
-      </c>
-      <c r="C70" t="n">
-        <v>1</v>
-      </c>
-      <c r="D70" t="n">
-        <v>126.1377666666667</v>
-      </c>
-      <c r="E70" t="n">
-        <v>0.2602581077827704</v>
-      </c>
-      <c r="F70" t="n">
-        <v>1200</v>
-      </c>
-      <c r="G70" t="n">
-        <v>151.2493100000001</v>
-      </c>
-      <c r="H70" t="n">
-        <v>0.7032402392548338</v>
-      </c>
-      <c r="I70" t="n">
-        <v>60.54266808444977</v>
-      </c>
-      <c r="J70" t="n">
-        <v>21.52416</v>
-      </c>
-      <c r="K70" t="n">
-        <v>20.03652</v>
-      </c>
-      <c r="L70" t="n">
-        <v>19.73887</v>
-      </c>
-      <c r="M70" t="n">
         <v>19.66344</v>
       </c>
     </row>

</xml_diff>